<commit_message>
Update training data and remove project status doc
Updated the training data Excel file and deleted the project status handover markdown document. The removal likely reflects a transition in project documentation or a completed handover.
</commit_message>
<xml_diff>
--- a/training/data/例文入力元_分解結果_v2_20250810_113552.xlsx
+++ b/training/data/例文入力元_分解結果_v2_20250810_113552.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\完全トレーニングUI完成フェーズ３\project-root\Rephrase-Project\training\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845A8A09-E007-4282-9BB2-022B6F01535F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C904726C-9DBE-42A7-AFB2-2662C8856645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3530" yWindow="3590" windowWidth="33490" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3570" yWindow="2870" windowWidth="33490" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="347">
   <si>
     <t>構文ID</t>
   </si>
@@ -1031,13 +1031,43 @@
   </si>
   <si>
     <t>proposal</t>
+  </si>
+  <si>
+    <t>完了形のhaveやhaven't、can, can'tなどのAuxのorderは正しいか。</t>
+  </si>
+  <si>
+    <t>can'tを正しく「can't」でスロットに入れているか（勝手にcan notにしていないか）</t>
+  </si>
+  <si>
+    <t>「You,」のような呼びかけが文頭にある場合のスロット選定（M1が正しい）は正しいか。</t>
+  </si>
+  <si>
+    <t>to himのようなto+目的格の副詞句はスロットに割り当てられているか（M2）</t>
+  </si>
+  <si>
+    <t>pleaseが文尾にあるとき、スロットに割り当てられているか（M3）</t>
+  </si>
+  <si>
+    <t>write it downのような目的語を真ん中に挟むタイプの句動詞で、downがスロットに割り当てられているか（M2）</t>
+  </si>
+  <si>
+    <t>her roomのように形容詞がついている名詞をそのままスロットに入れているか。herを省略していないか</t>
+  </si>
+  <si>
+    <t>a few days ago,for 2 yearsのような副詞において、agoをもう一度副詞としてカウントするなど重複、前置詞の欠落などは無いか</t>
+  </si>
+  <si>
+    <t>動詞を正しくV_group_keyに入力できているか</t>
+  </si>
+  <si>
+    <t>例文に対して分解後の要素が欠落しているものはないか（I love you.なのに分解後がyouだけ、など）</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1058,6 +1088,11 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1095,11 +1130,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1402,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L303"/>
+  <dimension ref="A1:P311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A264" workbookViewId="0">
-      <selection activeCell="N78" sqref="N78"/>
+    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
+      <selection activeCell="P309" sqref="P309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -9170,7 +9206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>1080</v>
       </c>
@@ -9196,7 +9232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>1080</v>
       </c>
@@ -9222,7 +9258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>1080</v>
       </c>
@@ -9248,7 +9284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>1081</v>
       </c>
@@ -9277,7 +9313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>1081</v>
       </c>
@@ -9303,7 +9339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>1081</v>
       </c>
@@ -9329,7 +9365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>1082</v>
       </c>
@@ -9358,7 +9394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>1082</v>
       </c>
@@ -9384,7 +9420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>1082</v>
       </c>
@@ -9410,7 +9446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>1083</v>
       </c>
@@ -9439,7 +9475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>1083</v>
       </c>
@@ -9465,7 +9501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>1083</v>
       </c>
@@ -9491,7 +9527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>1084</v>
       </c>
@@ -9520,7 +9556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:16" ht="14" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>1084</v>
       </c>
@@ -9545,8 +9581,11 @@
       <c r="K302">
         <v>0</v>
       </c>
-    </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="P302" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="303" spans="1:16" ht="14" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>1084</v>
       </c>
@@ -9570,10 +9609,54 @@
       </c>
       <c r="K303">
         <v>0</v>
+      </c>
+      <c r="P303" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="304" spans="1:16" ht="14" x14ac:dyDescent="0.3">
+      <c r="P304" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="305" spans="16:16" ht="14" x14ac:dyDescent="0.3">
+      <c r="P305" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="306" spans="16:16" ht="14" x14ac:dyDescent="0.3">
+      <c r="P306" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="307" spans="16:16" ht="14" x14ac:dyDescent="0.3">
+      <c r="P307" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="308" spans="16:16" ht="14" x14ac:dyDescent="0.3">
+      <c r="P308" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="309" spans="16:16" ht="14" x14ac:dyDescent="0.3">
+      <c r="P309" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="310" spans="16:16" ht="14" x14ac:dyDescent="0.3">
+      <c r="P310" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="311" spans="16:16" ht="14" x14ac:dyDescent="0.3">
+      <c r="P311" s="2" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>